<commit_message>
WIP fixing up pages
</commit_message>
<xml_diff>
--- a/budgetportal/tests/test_data/test_prov_infra_projects_empty_file.xlsx
+++ b/budgetportal/tests/test_data/test_prov_infra_projects_empty_file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="39">
   <si>
     <t xml:space="preserve">Project ID</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">Department</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sector</t>
   </si>
   <si>
     <t xml:space="preserve">Local Municipality</t>
@@ -244,16 +247,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:CH9"/>
+  <dimension ref="A1:CI9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CB1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CK1" activeCellId="0" sqref="CK1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -371,207 +371,210 @@
         <v>37</v>
       </c>
       <c r="AM1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AN1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AO1" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="AP1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AQ1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="AP1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="AR1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AS1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AT1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AU1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AV1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AW1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AX1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AY1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AZ1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BA1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BB1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BC1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BD1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BE1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BF1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BG1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BH1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BI1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BJ1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BK1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BL1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BM1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BN1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BO1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BP1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BQ1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BR1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BS1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BT1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BU1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BV1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BW1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BX1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BY1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BZ1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="CA1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="CB1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="CC1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="CD1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="CE1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="CF1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="CG1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="CH1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="CI1" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1"/>
-      <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1"/>
-      <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
-      <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1"/>
-      <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1"/>
-      <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
-      <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1"/>
-      <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1"/>
-      <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>